<commit_message>
Date and Time added to the location
</commit_message>
<xml_diff>
--- a/layouts/default/bulkuploadtitles.xlsx
+++ b/layouts/default/bulkuploadtitles.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>S No</t>
   </si>
@@ -29,7 +29,7 @@
     <t>Author</t>
   </si>
   <si>
-    <t>Circulation Status ( inactive, checked in,  Lost)</t>
+    <t>Circulation Status(inactive,checked in,lost)</t>
   </si>
   <si>
     <t>Category (Adult, Young, Child)</t>
@@ -44,7 +44,10 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Location Id</t>
+    <t>LocationId</t>
+  </si>
+  <si>
+    <t>Publication</t>
   </si>
 </sst>
 </file>
@@ -165,20 +168,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I2" activeCellId="0" pane="topLeft" sqref="I2"/>
+      <selection activeCell="D19" activeCellId="0" pane="topLeft" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.44313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="27.4588235294118"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.0039215686275"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.1019607843137"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="1" width="14.7529411764706"/>
-    <col collapsed="false" hidden="false" max="255" min="9" style="1" width="8.57254901960784"/>
-    <col collapsed="false" hidden="false" max="1025" min="256" style="1" width="11.9843137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.51764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="32.078431372549"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="38.7450980392157"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.3176470588235"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="1" width="14.9058823529412"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.078431372549"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.3607843137255"/>
+    <col collapsed="false" hidden="false" max="255" min="11" style="1" width="8.65490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="256" style="1" width="12.1098039215686"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="35.05" outlineLevel="0" r="1" s="4">
@@ -208,6 +213,9 @@
       </c>
       <c r="I1" s="3" t="s">
         <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>